<commit_message>
Draft partnership alignment class
</commit_message>
<xml_diff>
--- a/input/time_series_factor.xlsx
+++ b/input/time_series_factor.xlsx
@@ -5,25 +5,26 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F7DE037-E905-436A-9663-9E7932FCFF4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C6B955C-C95C-4F7B-86D7-E06C4B33BA2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
     <sheet name="UK_care_adjustment" sheetId="14" r:id="rId2"/>
-    <sheet name="UK_gdp" sheetId="2" r:id="rId3"/>
-    <sheet name="UK_inflation" sheetId="7" r:id="rId4"/>
-    <sheet name="UK_wage_growth" sheetId="8" r:id="rId5"/>
-    <sheet name="UK_saving_returns" sheetId="9" r:id="rId6"/>
-    <sheet name="UK_debt_cost_low" sheetId="10" r:id="rId7"/>
-    <sheet name="UK_debt_cost_hi" sheetId="11" r:id="rId8"/>
-    <sheet name="UK_carer_hourly_wage" sheetId="13" r:id="rId9"/>
-    <sheet name="UK raw data" sheetId="12" r:id="rId10"/>
-    <sheet name="IT" sheetId="4" r:id="rId11"/>
+    <sheet name="UK_cohabitation_adjustment" sheetId="15" r:id="rId3"/>
+    <sheet name="UK_gdp" sheetId="2" r:id="rId4"/>
+    <sheet name="UK_inflation" sheetId="7" r:id="rId5"/>
+    <sheet name="UK_wage_growth" sheetId="8" r:id="rId6"/>
+    <sheet name="UK_saving_returns" sheetId="9" r:id="rId7"/>
+    <sheet name="UK_debt_cost_low" sheetId="10" r:id="rId8"/>
+    <sheet name="UK_debt_cost_hi" sheetId="11" r:id="rId9"/>
+    <sheet name="UK_carer_hourly_wage" sheetId="13" r:id="rId10"/>
+    <sheet name="UK raw data" sheetId="12" r:id="rId11"/>
+    <sheet name="IT" sheetId="4" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -46,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="54">
   <si>
     <t>Year</t>
   </si>
@@ -620,6 +621,131 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C9E94E-195D-449C-95FA-8827E1CD938F}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>9.0451221008231997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3" s="7">
+        <v>9.1220556745181991</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4" s="7">
+        <v>8.9177939646201878</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5" s="7">
+        <v>8.7106598984771573</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6" s="7">
+        <v>8.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7" s="7">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8" s="7">
+        <v>9.1360476663356494</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9" s="7">
+        <v>9.2263056092843314</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10" s="7">
+        <v>9.3767705382436262</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11" s="7">
+        <v>9.6103896103896105</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12" s="7">
+        <v>9.9724011039558409</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13" s="7">
+        <v>9.9283154121863806</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14" s="7">
+        <v>10.012761014679809</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8E4EE1-1BD6-4E11-9F6E-85D51F484400}">
   <dimension ref="A1:BG120"/>
   <sheetViews>
@@ -8658,7 +8784,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB137BA4-4035-472D-AA2B-29C110ABC52B}">
   <dimension ref="A1:B74"/>
   <sheetViews>
@@ -9269,7 +9395,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6878765F-1722-41F9-8BBC-D6A1331F5260}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -9537,6 +9663,277 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18E90C-6D91-4744-9FCB-A05B59544AB8}">
+  <dimension ref="A1:B32"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>2010</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2011</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2012</v>
+      </c>
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>2013</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2014</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>2015</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>2016</v>
+      </c>
+      <c r="B8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>2017</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>2018</v>
+      </c>
+      <c r="B10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>2019</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2020</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>2021</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>2022</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>2023</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>2024</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>2025</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>2026</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>2027</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>2028</v>
+      </c>
+      <c r="B20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>2029</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>2030</v>
+      </c>
+      <c r="B22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>2031</v>
+      </c>
+      <c r="B23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>2032</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>2033</v>
+      </c>
+      <c r="B25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>2034</v>
+      </c>
+      <c r="B26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>2035</v>
+      </c>
+      <c r="B27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>2036</v>
+      </c>
+      <c r="B28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>2037</v>
+      </c>
+      <c r="B29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>2038</v>
+      </c>
+      <c r="B30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>2039</v>
+      </c>
+      <c r="B31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>2040</v>
+      </c>
+      <c r="B32">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5368A556-88DB-4602-9465-944BD364475C}">
   <dimension ref="A1:B116"/>
   <sheetViews>
@@ -10479,7 +10876,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2B7FF6-C3ED-409F-83AB-FB5EAD53E39E}">
   <dimension ref="A1:B42"/>
   <sheetViews>
@@ -10831,7 +11228,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F3F720F-7C77-40C9-9D26-48C5FF4C5828}">
   <dimension ref="A1:B30"/>
   <sheetViews>
@@ -11086,7 +11483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE1C571-12D2-48EC-9676-C9293E844074}">
   <dimension ref="A1:B38"/>
   <sheetViews>
@@ -11405,7 +11802,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF70C8B1-8A2A-4CB2-AE85-70911F99E869}">
   <dimension ref="A1:B30"/>
   <sheetViews>
@@ -11660,7 +12057,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE5D1202-306C-4A3E-BE31-47D9872C9300}">
   <dimension ref="A1:B30"/>
   <sheetViews>
@@ -11913,129 +12310,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C9E94E-195D-449C-95FA-8827E1CD938F}">
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>2010</v>
-      </c>
-      <c r="B2">
-        <v>9.0451221008231997</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2011</v>
-      </c>
-      <c r="B3" s="7">
-        <v>9.1220556745181991</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>2012</v>
-      </c>
-      <c r="B4" s="7">
-        <v>8.9177939646201878</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <v>2013</v>
-      </c>
-      <c r="B5" s="7">
-        <v>8.7106598984771573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2014</v>
-      </c>
-      <c r="B6" s="7">
-        <v>8.58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>2015</v>
-      </c>
-      <c r="B7" s="7">
-        <v>8.7899999999999991</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>2016</v>
-      </c>
-      <c r="B8" s="7">
-        <v>9.1360476663356494</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>2017</v>
-      </c>
-      <c r="B9" s="7">
-        <v>9.2263056092843314</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>2018</v>
-      </c>
-      <c r="B10" s="7">
-        <v>9.3767705382436262</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>2019</v>
-      </c>
-      <c r="B11" s="7">
-        <v>9.6103896103896105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>2020</v>
-      </c>
-      <c r="B12" s="7">
-        <v>9.9724011039558409</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>2021</v>
-      </c>
-      <c r="B13" s="7">
-        <v>9.9283154121863806</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>2022</v>
-      </c>
-      <c r="B14" s="7">
-        <v>10.012761014679809</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
amendments to model during calibration
</commit_message>
<xml_diff>
--- a/input/time_series_factor.xlsx
+++ b/input/time_series_factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patryk\git\SimPathsFork\input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E3C59E3-D303-406A-B429-72CAA160EF3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2230FFC2-34A8-41AA-8CD2-76BFCA066129}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -29,28 +29,17 @@
     <sheet name="UK raw data" sheetId="12" r:id="rId14"/>
     <sheet name="IT" sheetId="4" r:id="rId15"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="54">
   <si>
     <t>Year</t>
   </si>
@@ -122,9 +111,6 @@
   </si>
   <si>
     <t>Bank of England website</t>
-  </si>
-  <si>
-    <t>GDP CVMs</t>
   </si>
   <si>
     <t>ONS variable YBEZ</t>
@@ -212,6 +198,9 @@
   </si>
   <si>
     <t>NOMINAL</t>
+  </si>
+  <si>
+    <t>GDP CVMs (real)</t>
   </si>
 </sst>
 </file>
@@ -571,8 +560,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -583,39 +572,42 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" t="s">
         <v>44</v>
-      </c>
-      <c r="B6" t="s">
-        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -627,9 +619,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AE1C571-12D2-48EC-9676-C9293E844074}">
   <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B38"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -947,7 +937,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1202,7 +1192,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1456,7 +1446,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A4C9E94E-195D-449C-95FA-8827E1CD938F}">
   <dimension ref="A1:B14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1581,8 +1573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E8E4EE1-1BD6-4E11-9F6E-85D51F484400}">
   <dimension ref="A1:BG120"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
-      <selection activeCell="AR28" sqref="AR28"/>
+    <sheetView topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AV2" sqref="AV2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1620,7 +1612,7 @@
       <c r="Y1" s="4"/>
       <c r="Z1" s="4"/>
       <c r="AB1" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
@@ -1637,19 +1629,19 @@
       <c r="AN1" s="4"/>
       <c r="AO1" s="4"/>
       <c r="AQ1" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="AR1" s="4"/>
       <c r="AS1" s="4"/>
       <c r="AT1" s="4"/>
       <c r="AV1" s="4" t="s">
-        <v>24</v>
+        <v>53</v>
       </c>
       <c r="AW1" s="4"/>
       <c r="AX1" s="4"/>
       <c r="AY1" s="4"/>
       <c r="BA1" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="BB1" s="4"/>
       <c r="BC1" s="4"/>
@@ -1666,7 +1658,7 @@
         <v>11</v>
       </c>
       <c r="J2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="X2" t="s">
         <v>12</v>
@@ -1678,22 +1670,22 @@
         <v>14</v>
       </c>
       <c r="AQ2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AV2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="AX2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AY2" t="s">
         <v>32</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>33</v>
       </c>
       <c r="BA2" t="s">
         <v>2</v>
       </c>
       <c r="BB2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:56" x14ac:dyDescent="0.25">
@@ -1704,17 +1696,17 @@
         <v>16</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F3" s="10"/>
       <c r="K3" t="s">
         <v>16</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="M3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="N3" s="10"/>
       <c r="Q3" t="s">
@@ -1736,7 +1728,7 @@
         <v>22</v>
       </c>
       <c r="AE3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AF3" s="10"/>
       <c r="AI3" t="s">
@@ -1746,27 +1738,27 @@
         <v>23</v>
       </c>
       <c r="AM3" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="AN3" s="10"/>
       <c r="AO3" s="10"/>
       <c r="AQ3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AS3" s="10" t="s">
         <v>48</v>
-      </c>
-      <c r="AS3" s="10" t="s">
-        <v>49</v>
       </c>
       <c r="AT3" s="10"/>
       <c r="BA3" t="s">
         <v>3</v>
       </c>
       <c r="BB3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <f>MIN(A8:A156)</f>
@@ -1779,7 +1771,7 @@
       <c r="E4" s="10"/>
       <c r="F4" s="10"/>
       <c r="J4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4">
         <f>MIN(H8:H156)</f>
@@ -1792,30 +1784,30 @@
       <c r="M4" s="10"/>
       <c r="N4" s="10"/>
       <c r="AC4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AD4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AE4" s="10"/>
       <c r="AF4" s="10"/>
       <c r="AI4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AJ4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AK4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AL4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="AM4" s="10"/>
       <c r="AN4" s="10"/>
       <c r="AO4" s="10"/>
       <c r="AQ4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AR4">
         <f>(AT19/AT9)^(1/(AQ19-AQ9))</f>
@@ -1824,7 +1816,7 @@
       <c r="AS4" s="10"/>
       <c r="AT4" s="10"/>
       <c r="AV4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="AW4">
         <f>MIN(AV8:AV156)</f>
@@ -1841,7 +1833,7 @@
     </row>
     <row r="5" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B5">
         <f>MAX(A8:A156)</f>
@@ -1854,7 +1846,7 @@
       <c r="E5" s="10"/>
       <c r="F5" s="10"/>
       <c r="J5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="K5">
         <f>MAX(H8:H156)</f>
@@ -1874,7 +1866,7 @@
       <c r="AS5" s="10"/>
       <c r="AT5" s="10"/>
       <c r="AV5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="AW5">
         <f>MAX(AV8:AV156)</f>
@@ -1890,7 +1882,7 @@
     </row>
     <row r="6" spans="1:56" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C6">
         <f>(C5/C4)^(1/(B5-B4))</f>
@@ -1899,7 +1891,7 @@
       <c r="E6" s="10"/>
       <c r="F6" s="10"/>
       <c r="J6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L6">
         <f>(L5/L4)^(1/(K5-K4))</f>
@@ -1908,7 +1900,7 @@
       <c r="M6" s="10"/>
       <c r="N6" s="10"/>
       <c r="AB6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AC6">
         <f>AVERAGE(AC9:AC82)</f>
@@ -1921,7 +1913,7 @@
       <c r="AE6" s="10"/>
       <c r="AF6" s="10"/>
       <c r="AJ6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AK6">
         <f>AVERAGE(AK9:AK82)</f>
@@ -1935,11 +1927,11 @@
       <c r="AN6" s="10"/>
       <c r="AO6" s="10"/>
       <c r="AR6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="AS6" s="10"/>
       <c r="AT6" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:56" x14ac:dyDescent="0.25">
@@ -5266,7 +5258,7 @@
         <v>13.459023539668697</v>
       </c>
       <c r="BF28" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG28">
         <f t="shared" ref="BG28:BG59" si="46">BA28</f>
@@ -5431,7 +5423,7 @@
         <v>12.768817204301072</v>
       </c>
       <c r="BF29" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG29">
         <f t="shared" si="46"/>
@@ -5594,7 +5586,7 @@
         <v>11.999611348620284</v>
       </c>
       <c r="BF30" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG30">
         <f t="shared" si="46"/>
@@ -5757,7 +5749,7 @@
         <v>10.944700460829491</v>
       </c>
       <c r="BF31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG31">
         <f t="shared" si="46"/>
@@ -5920,7 +5912,7 @@
         <v>10.267708679747255</v>
       </c>
       <c r="BF32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG32">
         <f t="shared" si="46"/>
@@ -6083,7 +6075,7 @@
         <v>9.3959220937309773</v>
       </c>
       <c r="BF33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG33">
         <f t="shared" si="46"/>
@@ -6246,7 +6238,7 @@
         <v>7.9045058883768542</v>
       </c>
       <c r="BF34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG34">
         <f t="shared" si="46"/>
@@ -6394,7 +6386,7 @@
         <v>6.4255983350676367</v>
       </c>
       <c r="BF35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG35">
         <f t="shared" si="46"/>
@@ -6516,7 +6508,7 @@
         <v>5.5331541218637987</v>
       </c>
       <c r="BF36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG36">
         <f t="shared" si="46"/>
@@ -6626,7 +6618,7 @@
         <v>4.788306451612903</v>
       </c>
       <c r="BF37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG37">
         <f t="shared" si="46"/>
@@ -6736,7 +6728,7 @@
         <v>4.368279569892473</v>
       </c>
       <c r="BF38" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG38">
         <f t="shared" si="46"/>
@@ -6846,7 +6838,7 @@
         <v>3.8306451612903225</v>
       </c>
       <c r="BF39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG39">
         <f t="shared" si="46"/>
@@ -6956,7 +6948,7 @@
         <v>3.276209677419355</v>
       </c>
       <c r="BF40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG40">
         <f t="shared" si="46"/>
@@ -7066,7 +7058,7 @@
         <v>2.920726515939835</v>
       </c>
       <c r="BF41" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG41">
         <f t="shared" si="46"/>
@@ -7177,7 +7169,7 @@
         <v>2.6701548041165788</v>
       </c>
       <c r="BF42" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG42">
         <f t="shared" si="46"/>
@@ -7285,7 +7277,7 @@
         <v>2.5214373213556551</v>
       </c>
       <c r="BF43" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG43">
         <f t="shared" si="46"/>
@@ -7371,7 +7363,7 @@
         <v>2.3941532258064511</v>
       </c>
       <c r="BF44" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG44">
         <f t="shared" si="46"/>
@@ -7448,7 +7440,7 @@
         <v>2.3001564478879533</v>
       </c>
       <c r="BF45" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG45">
         <f t="shared" si="46"/>
@@ -7525,7 +7517,7 @@
         <v>2.2083541949788996</v>
       </c>
       <c r="BF46" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG46">
         <f t="shared" si="46"/>
@@ -7592,7 +7584,7 @@
         <v>2.1190803019903908</v>
       </c>
       <c r="BF47" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG47">
         <f t="shared" si="46"/>
@@ -7650,7 +7642,7 @@
         <v>2.0161290322580645</v>
       </c>
       <c r="BF48" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG48">
         <f t="shared" si="46"/>
@@ -7708,7 +7700,7 @@
         <v>1.9157088122605364</v>
       </c>
       <c r="BF49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG49">
         <f t="shared" si="46"/>
@@ -7768,7 +7760,7 @@
         <v>1.7889087656529516</v>
       </c>
       <c r="BF50" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG50">
         <f t="shared" si="46"/>
@@ -7828,7 +7820,7 @@
         <v>1.6638935108153077</v>
       </c>
       <c r="BF51" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG51">
         <f t="shared" si="46"/>
@@ -7876,7 +7868,7 @@
         <v>1.5974440894568689</v>
       </c>
       <c r="BF52" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG52">
         <f t="shared" si="46"/>
@@ -7924,7 +7916,7 @@
         <v>1.557632398753894</v>
       </c>
       <c r="BF53" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG53">
         <f t="shared" si="46"/>
@@ -7972,7 +7964,7 @@
         <v>1.5267175572519085</v>
       </c>
       <c r="BF54" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG54">
         <f t="shared" si="46"/>
@@ -8020,7 +8012,7 @@
         <v>1.4880952380952381</v>
       </c>
       <c r="BF55" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG55">
         <f t="shared" si="46"/>
@@ -8068,7 +8060,7 @@
         <v>1.4534883720930234</v>
       </c>
       <c r="BF56" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG56">
         <f t="shared" si="46"/>
@@ -8116,7 +8108,7 @@
         <v>1.4265335235378032</v>
       </c>
       <c r="BF57" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG57">
         <f t="shared" si="46"/>
@@ -8164,7 +8156,7 @@
         <v>1.4044943820224718</v>
       </c>
       <c r="BF58" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG58">
         <f t="shared" si="46"/>
@@ -8212,7 +8204,7 @@
         <v>1.3869625520110958</v>
       </c>
       <c r="BF59" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG59">
         <f t="shared" si="46"/>
@@ -8260,7 +8252,7 @@
         <v>1.3755158184319118</v>
       </c>
       <c r="BF60" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG60">
         <f t="shared" ref="BG60:BG81" si="59">BA60</f>
@@ -8298,7 +8290,7 @@
         <v>1.3586956521739131</v>
       </c>
       <c r="BF61" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG61">
         <f t="shared" si="59"/>
@@ -8336,7 +8328,7 @@
         <v>1.3422818791946309</v>
       </c>
       <c r="BF62" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG62">
         <f t="shared" si="59"/>
@@ -8374,7 +8366,7 @@
         <v>1.3245033112582782</v>
       </c>
       <c r="BF63" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG63">
         <f t="shared" si="59"/>
@@ -8412,7 +8404,7 @@
         <v>1.3071895424836601</v>
       </c>
       <c r="BF64" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG64">
         <f t="shared" si="59"/>
@@ -8450,7 +8442,7 @@
         <v>1.2804097311139566</v>
       </c>
       <c r="BF65" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG65">
         <f t="shared" si="59"/>
@@ -8488,7 +8480,7 @@
         <v>1.2515644555694618</v>
       </c>
       <c r="BF66" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG66">
         <f t="shared" si="59"/>
@@ -8526,7 +8518,7 @@
         <v>1.2224938875305624</v>
       </c>
       <c r="BF67" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG67">
         <f t="shared" si="59"/>
@@ -8564,7 +8556,7 @@
         <v>1.1806375442739079</v>
       </c>
       <c r="BF68" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG68">
         <f t="shared" si="59"/>
@@ -8602,7 +8594,7 @@
         <v>1.1547344110854505</v>
       </c>
       <c r="BF69" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG69">
         <f t="shared" si="59"/>
@@ -8640,7 +8632,7 @@
         <v>1.1185682326621924</v>
       </c>
       <c r="BF70" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG70">
         <f t="shared" si="59"/>
@@ -8678,7 +8670,7 @@
         <v>1.070663811563169</v>
       </c>
       <c r="BF71" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG71">
         <f t="shared" si="59"/>
@@ -8716,7 +8708,7 @@
         <v>1.0405827263267431</v>
       </c>
       <c r="BF72" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG72">
         <f t="shared" si="59"/>
@@ -8754,7 +8746,7 @@
         <v>1.015228426395939</v>
       </c>
       <c r="BF73" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG73">
         <f t="shared" si="59"/>
@@ -8792,7 +8784,7 @@
         <v>1</v>
       </c>
       <c r="BF74" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG74">
         <f t="shared" si="59"/>
@@ -8830,7 +8822,7 @@
         <v>1</v>
       </c>
       <c r="BF75" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG75">
         <f t="shared" si="59"/>
@@ -8868,7 +8860,7 @@
         <v>0.99304865938430975</v>
       </c>
       <c r="BF76" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG76">
         <f t="shared" si="59"/>
@@ -8906,7 +8898,7 @@
         <v>0.96711798839458407</v>
       </c>
       <c r="BF77" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG77">
         <f t="shared" si="59"/>
@@ -8944,7 +8936,7 @@
         <v>0.94428706326723322</v>
       </c>
       <c r="BF78" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG78">
         <f t="shared" si="59"/>
@@ -8982,7 +8974,7 @@
         <v>0.927643784786642</v>
       </c>
       <c r="BF79" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG79">
         <f t="shared" si="59"/>
@@ -9020,7 +9012,7 @@
         <v>0.91996320147194111</v>
       </c>
       <c r="BF80" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG80">
         <f t="shared" si="59"/>
@@ -9058,7 +9050,7 @@
         <v>0.89605734767025091</v>
       </c>
       <c r="BF81" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="BG81">
         <f t="shared" si="59"/>
@@ -10228,7 +10220,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10499,7 +10491,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10770,7 +10762,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11041,7 +11033,7 @@
   <dimension ref="A1:B32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11311,8 +11303,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A8B1C6-B095-49F5-BE52-65A3AD804239}">
   <dimension ref="A1:B32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11582,8 +11574,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5368A556-88DB-4602-9465-944BD364475C}">
   <dimension ref="A1:B116"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="B116" sqref="B116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12525,8 +12517,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC2B7FF6-C3ED-409F-83AB-FB5EAD53E39E}">
   <dimension ref="A1:B42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B42"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12878,7 +12870,7 @@
   <dimension ref="A1:B30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new object to align starting population with targets
</commit_message>
<xml_diff>
--- a/input/time_series_factor.xlsx
+++ b/input/time_series_factor.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADBD0E3-201F-48D3-8C6E-04F0B8687273}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF57C219-12C7-498D-BE53-E1D94A803CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -10746,8 +10746,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18E90C-6D91-4744-9FCB-A05B59544AB8}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G36" sqref="G36"/>
+    <sheetView topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10845,7 +10845,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10853,7 +10853,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>-1.6569848738871</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10861,7 +10861,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>-1.96530789753477</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10869,7 +10869,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>-1.6296433777680699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10877,7 +10877,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>-1.61360197486796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10885,7 +10885,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>-1.6349730701249401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10893,7 +10893,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>-1.5445370637206699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10901,7 +10901,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>-1.4299905126036001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10909,7 +10909,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>-1.3400796721802499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -10917,7 +10917,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>-1.3976698241718599</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -10925,7 +10925,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>-1.4046510893805899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -10933,7 +10933,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>-1.5186778343693299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -10941,7 +10941,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>-1.2394763356524801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -10949,7 +10949,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>-1.42824525283615</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -10957,7 +10957,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>-1.2868269051383801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -10965,7 +10965,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>-1.2949964344101601</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -10973,7 +10973,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>-1.43938829517986</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -10981,7 +10981,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>-1.36232927536807</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -10989,7 +10989,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>-1.3787822543156101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -10997,7 +10997,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>-1.0279518813227599</v>
+        <v>0</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -11005,7 +11005,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>-1.01288583307878</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -11013,7 +11013,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>-1.0374046613319601</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -11021,7 +11021,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>-1.0737369738603599</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -11029,7 +11029,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>-0.92895912934229796</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -11037,7 +11037,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>-0.90507790568283197</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -11045,7 +11045,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>-0.96147783613818705</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -11053,7 +11053,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>-1.0137664043043999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -11061,7 +11061,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>-1.0337977225364501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -11069,7 +11069,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>-0.97418124454538801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -11077,7 +11077,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>-1.0654412312299</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -11085,7 +11085,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>-1.2965068712400101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -11093,7 +11093,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>-1.1196723042102801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -11101,7 +11101,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>-1.09930572758417</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -11109,7 +11109,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>-1.11186657756847</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -11117,7 +11117,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>-1.1437646981801199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -11125,7 +11125,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>-1.0609547215406401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -11133,7 +11133,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>-1.12208261153533</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -11141,7 +11141,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>-1.1819933852217499</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -11149,7 +11149,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>-1.1092094630354199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -11157,7 +11157,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>-1.2921210311593401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -11165,7 +11165,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>-1.22126428849136</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -11173,7 +11173,7 @@
         <v>2061</v>
       </c>
       <c r="B53">
-        <v>-1.0633265041651601</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -11181,7 +11181,7 @@
         <v>2062</v>
       </c>
       <c r="B54">
-        <v>-0.98841225305358904</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -11189,7 +11189,7 @@
         <v>2063</v>
       </c>
       <c r="B55">
-        <v>-1.1774351160324801</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -11197,7 +11197,7 @@
         <v>2064</v>
       </c>
       <c r="B56">
-        <v>-1.2024231783985999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -11205,7 +11205,7 @@
         <v>2065</v>
       </c>
       <c r="B57">
-        <v>-1.0864234009210501</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -11213,7 +11213,7 @@
         <v>2066</v>
       </c>
       <c r="B58">
-        <v>-0.93974029584678198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -11221,7 +11221,7 @@
         <v>2067</v>
       </c>
       <c r="B59">
-        <v>-0.97940174059324703</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -11229,7 +11229,7 @@
         <v>2068</v>
       </c>
       <c r="B60">
-        <v>-1.07489350785768</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -11237,7 +11237,7 @@
         <v>2069</v>
       </c>
       <c r="B61">
-        <v>-1.10747132686233</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -11249,7 +11249,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00E6D01-ED8F-4196-BCE1-0F54EC92EC33}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B61"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -11346,7 +11348,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>-0.35953928067081697</v>
+        <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -11354,7 +11356,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>-0.332777758808455</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -11362,7 +11364,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>-0.31361348135702599</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -11370,7 +11372,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>-0.30467159374472402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -11378,7 +11380,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>-0.33311666105385201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -11386,7 +11388,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>-0.114065941244585</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -11394,7 +11396,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>-0.184749066479824</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -11402,7 +11404,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>-0.50743389410911699</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11418,7 +11420,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>-0.169774412346757</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -11426,7 +11428,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>-0.22569190327833999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -11434,7 +11436,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>-0.20877695406551899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -11450,7 +11452,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>-4.9138528269517097E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -11466,7 +11468,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>-0.135473612417048</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -11474,7 +11476,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>-0.15436967579529001</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -11482,7 +11484,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>-0.24139950566465199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -11490,7 +11492,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>-0.137551024781153</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -11506,7 +11508,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>-0.35728162191093199</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -11514,7 +11516,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>-0.16740709219885999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -11522,7 +11524,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>-0.194350213772646</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -11530,7 +11532,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>-0.148012953985378</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -11538,7 +11540,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>-0.46412058506835702</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -11546,7 +11548,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>-0.17308002089213401</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -11554,7 +11556,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>-0.32803567814586498</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -11562,7 +11564,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>-0.24886506276926701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -11570,7 +11572,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>-0.38900984398442701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -11578,7 +11580,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>-0.29714528858794198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -11586,7 +11588,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>-7.9059617090519799E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -11594,7 +11596,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>-0.13959658611456899</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -11602,7 +11604,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>-0.31091239479402999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -11610,7 +11612,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>-0.265724066343548</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -11618,7 +11620,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>-0.157973466853217</v>
+        <v>0</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -11626,7 +11628,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>-0.29504339957888198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -11634,7 +11636,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>-0.176402201753564</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -11642,7 +11644,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>-0.166209923745262</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -11650,7 +11652,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>-0.26649635719242798</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -11658,7 +11660,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>-0.188067583435434</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -11666,7 +11668,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>-0.33255975011313099</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -11674,7 +11676,7 @@
         <v>2061</v>
       </c>
       <c r="B53">
-        <v>-0.36686564218953999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -11682,7 +11684,7 @@
         <v>2062</v>
       </c>
       <c r="B54">
-        <v>-0.27733798163249901</v>
+        <v>0</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -11690,7 +11692,7 @@
         <v>2063</v>
       </c>
       <c r="B55">
-        <v>-0.35401505108231701</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -11698,7 +11700,7 @@
         <v>2064</v>
       </c>
       <c r="B56">
-        <v>-0.25048354603053402</v>
+        <v>0</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -11706,7 +11708,7 @@
         <v>2065</v>
       </c>
       <c r="B57">
-        <v>-0.222960408429973</v>
+        <v>0</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -11714,7 +11716,7 @@
         <v>2066</v>
       </c>
       <c r="B58">
-        <v>-0.28035343751848202</v>
+        <v>0</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -11722,7 +11724,7 @@
         <v>2067</v>
       </c>
       <c r="B59">
-        <v>-6.4311567615268794E-2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -11730,7 +11732,7 @@
         <v>2068</v>
       </c>
       <c r="B60">
-        <v>-0.27562599475480198</v>
+        <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -11738,7 +11740,7 @@
         <v>2069</v>
       </c>
       <c r="B61">
-        <v>-0.28048846572702102</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
variant 2 for social care analysis
</commit_message>
<xml_diff>
--- a/input/time_series_factor.xlsx
+++ b/input/time_series_factor.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF57C219-12C7-498D-BE53-E1D94A803CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32CF2CF9-CDA0-4325-8B5F-C2138C8D0814}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -10746,9 +10746,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18E90C-6D91-4744-9FCB-A05B59544AB8}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B61"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10845,7 +10843,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-1.70385500364881</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10853,7 +10851,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-1.1571997465369599</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10861,7 +10859,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-1.80929478189082</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10869,7 +10867,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>-1.45740161376961</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10877,7 +10875,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>-1.29073044690233</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10885,7 +10883,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>-1.3056634031600001</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10893,7 +10891,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>-1.23057408899539</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10901,7 +10899,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>-1.22857101286559</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10909,7 +10907,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>-1.1826767128946001</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -10917,7 +10915,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>-1.1579759478193301</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -10925,7 +10923,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>-1.12963486475958</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -10933,7 +10931,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-1.0757812715078701</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -10941,7 +10939,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>-1.12092793449733</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -10949,7 +10947,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>-1.1018731590873201</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -10957,7 +10955,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>-1.09760958793781</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -10965,7 +10963,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-1.0830768496758301</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -10973,7 +10971,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>-1.0555063329510599</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -10981,7 +10979,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>-1.0479160285220399</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -10989,7 +10987,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-1.0514706039277</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -10997,7 +10995,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>-1.06908691107647</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -11005,7 +11003,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-1.0415116257308501</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -11013,7 +11011,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-1.0513753123935701</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -11021,7 +11019,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>-1.04265085219326</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -11029,7 +11027,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-1.0414216342656399</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -11037,7 +11035,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>-1.0324540674931599</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -11045,7 +11043,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-1.02569115746613</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -11053,7 +11051,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-1.02695584627324</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -11061,7 +11059,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>-1.02822328009438</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -11069,7 +11067,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>-1.0256289303811199</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -11077,7 +11075,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>-1.01431235476579</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -11085,7 +11083,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>-1.0189988164694199</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -11093,7 +11091,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>-0.93569233126322005</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -11101,7 +11099,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>-1.0965571763798101</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -11109,7 +11107,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-1.0328666908366799</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -11117,7 +11115,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>-1.0312928178387699</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -11125,7 +11123,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>-1.0409650808786699</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -11133,7 +11131,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>-1.0051876412406699</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -11141,7 +11139,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>-1.0203281201491501</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -11149,7 +11147,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-1.0024476094547801</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -11157,7 +11155,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>-0.99635378684264198</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -11165,7 +11163,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>-1.01498858055898</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -11173,7 +11171,7 @@
         <v>2061</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>-1.0402525118708299</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -11181,7 +11179,7 @@
         <v>2062</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>-0.99703465162276605</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -11189,7 +11187,7 @@
         <v>2063</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>-1.0075997527413501</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -11197,7 +11195,7 @@
         <v>2064</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>-0.96736979634708398</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -11205,7 +11203,7 @@
         <v>2065</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>-0.95097258952846597</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -11213,7 +11211,7 @@
         <v>2066</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>-0.94182162387448598</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -11221,7 +11219,7 @@
         <v>2067</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>-0.99147068097634095</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -11229,7 +11227,7 @@
         <v>2068</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>-0.93307533098083895</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -11237,7 +11235,7 @@
         <v>2069</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>-0.94063451050118296</v>
       </c>
     </row>
   </sheetData>
@@ -11249,9 +11247,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00E6D01-ED8F-4196-BCE1-0F54EC92EC33}">
   <dimension ref="A1:B61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B61"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -11348,7 +11344,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-0.46934212296623401</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -11356,7 +11352,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-0.454739741051573</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -11364,7 +11360,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-0.38374565123458099</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -11372,7 +11368,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>-0.36783896829080098</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -11380,7 +11376,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>-0.33165493609233199</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -11388,7 +11384,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>-0.291562375123395</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -11396,7 +11392,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>-0.25198600505337698</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -11404,7 +11400,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>-0.28483236661986799</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11412,7 +11408,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>-0.19968626665699099</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -11420,7 +11416,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>-0.18811664205453299</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -11428,7 +11424,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>-0.19600519076745501</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -11436,7 +11432,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-0.170825426649971</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -11444,7 +11440,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>-0.180453640042601</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -11452,7 +11448,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>-0.16804309294200601</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -11460,7 +11456,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>-0.17399727223845801</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -11468,7 +11464,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-0.17239504964128299</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -11476,7 +11472,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>-0.190003699937489</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -11484,7 +11480,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>-0.20430272643120501</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -11492,7 +11488,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-0.175676089303543</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -11500,7 +11496,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>-0.20998728649817899</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -11508,7 +11504,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-0.203331600424143</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -11516,7 +11512,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-0.21884376646789699</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -11524,7 +11520,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>-0.23494724441978199</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -11532,7 +11528,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-0.203708135524758</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -11540,7 +11536,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>-0.21974647037595901</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -11548,7 +11544,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-0.22176718155054601</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -11556,7 +11552,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-0.216239660869704</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -11564,7 +11560,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>-0.234189632538475</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -11572,7 +11568,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>-0.20718286006263001</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -11580,7 +11576,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>-0.24936479477594001</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -11588,7 +11584,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>-0.22625695535786999</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -11596,7 +11592,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>-0.22193325066712699</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -11604,7 +11600,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>-0.255926102036931</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -11612,7 +11608,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-0.215144807846602</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -11620,7 +11616,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>-0.205975543344144</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -11628,7 +11624,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>-0.22623264483573799</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -11636,7 +11632,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>-0.21071425092177301</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -11644,7 +11640,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>-0.223422932715302</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -11652,7 +11648,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-0.241519153733185</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -11660,7 +11656,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>-0.22311606421336</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -11668,7 +11664,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>-0.247279492286858</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -11676,7 +11672,7 @@
         <v>2061</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>-0.225909829302193</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -11684,7 +11680,7 @@
         <v>2062</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>-0.21378817134198899</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -11692,7 +11688,7 @@
         <v>2063</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>-0.22796885539012501</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -11700,7 +11696,7 @@
         <v>2064</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>-0.23952823907995999</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -11708,7 +11704,7 @@
         <v>2065</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>-0.23200492090432101</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -11716,7 +11712,7 @@
         <v>2066</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>-0.25071493326128902</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -11724,7 +11720,7 @@
         <v>2067</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>-0.22327190713982001</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -11732,7 +11728,7 @@
         <v>2068</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>-0.22850366385618201</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -11740,7 +11736,7 @@
         <v>2069</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>-0.21569328218244499</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adjusted fertility and cohabitation alignment parmeters
Start social care calibration of utility parameters
</commit_message>
<xml_diff>
--- a/input/time_series_factor.xlsx
+++ b/input/time_series_factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50697902-4BEF-47A6-9571-C8E998A4ADC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097CE548-6F17-4B75-8319-73D61F0113A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
     <sheet name="UK raw data" sheetId="12" r:id="rId15"/>
     <sheet name="IT" sheetId="4" r:id="rId16"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -38,12 +38,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -223,7 +218,7 @@
     <numFmt numFmtId="164" formatCode="0.0"/>
     <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -237,8 +232,135 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri Light"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,8 +379,181 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -266,9 +561,157 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -291,8 +734,49 @@
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -10753,11 +11237,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18E90C-6D91-4744-9FCB-A05B59544AB8}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B61"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -10790,7 +11272,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-0.95768509819680903</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -10798,7 +11280,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-0.83295781453007001</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -10806,7 +11288,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>-0.80485660959326355</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -10814,7 +11296,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>-0.78981867057924415</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -10822,7 +11304,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-0.77794475503792282</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -10830,7 +11312,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-0.75171647264083308</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -10838,7 +11320,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-0.74109647439251236</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -10846,7 +11328,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-0.72776510107134573</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -10854,7 +11336,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-0.7147060419149136</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -10862,7 +11344,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-0.70240616614065376</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -10870,7 +11352,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-0.69105367590666433</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -10878,7 +11360,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>-0.67898522305967135</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -10886,7 +11368,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>-0.67837200227633576</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -10894,7 +11376,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>-0.66865521484219381</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -10902,7 +11384,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>-0.66213777125088935</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -10910,7 +11392,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>-0.65624918555298262</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -10918,7 +11400,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>-0.65247439548232655</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -10926,7 +11408,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>-0.64776174741668557</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -10934,7 +11416,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>-0.64184148070049241</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -10942,7 +11424,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-0.63931566276826524</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -10950,7 +11432,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>-0.63638760354965007</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -10958,7 +11440,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>-0.63218797948615213</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -10966,7 +11448,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>-0.62979949109872213</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -10974,7 +11456,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-0.62642840586058846</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -10982,7 +11464,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>-0.62703195252281929</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -10990,7 +11472,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>-0.62763592693798487</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -10998,7 +11480,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-0.62901387736233438</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -11006,7 +11488,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>-0.62870490298773551</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -11014,7 +11496,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-0.63132275325212173</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -11022,7 +11504,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-0.63189417814259741</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -11030,7 +11512,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>-0.63431628626780423</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -11038,7 +11520,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-0.63319756552905415</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -11046,7 +11528,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>-0.63471667603087323</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -11054,7 +11536,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-0.63455648067220116</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -11062,7 +11544,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-0.63527012935003857</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -11070,7 +11552,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>-0.63488663198137396</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -11078,7 +11560,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>-0.6327623871436846</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -11086,7 +11568,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>-0.63172645653828041</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -11094,7 +11576,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>-0.63131309782462763</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -11102,7 +11584,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>-0.62711212192261312</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -11110,7 +11592,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>-0.62483324297863929</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -11118,7 +11600,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-0.62289315139452228</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -11126,7 +11608,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>-0.6208575795852076</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -11134,7 +11616,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>-0.62046331508145192</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -11142,7 +11624,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>-0.61860426418741976</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -11150,7 +11632,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>-0.61533367788355553</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -11158,7 +11640,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-0.61489963029454253</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -11166,7 +11648,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>-0.61364330813003531</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -11174,7 +11656,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>-0.61242239408296961</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -11182,7 +11664,7 @@
         <v>2061</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>-0.61091556383364465</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -11190,7 +11672,7 @@
         <v>2062</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>-0.60932285274850906</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -11198,7 +11680,7 @@
         <v>2063</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>-0.60791630071486702</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -11206,7 +11688,7 @@
         <v>2064</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>-0.60902347078757146</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -11214,7 +11696,7 @@
         <v>2065</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>-0.60734177454365323</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -11222,7 +11704,7 @@
         <v>2066</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>-0.60672079418846891</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -11230,7 +11712,7 @@
         <v>2067</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>-0.6058496118125366</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -11238,7 +11720,7 @@
         <v>2068</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>-0.60652410750329455</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -11246,7 +11728,15 @@
         <v>2069</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>-0.60652410750329455</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2070</v>
+      </c>
+      <c r="B62">
+        <v>-0.60652410750329455</v>
       </c>
     </row>
   </sheetData>
@@ -11256,11 +11746,9 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00E6D01-ED8F-4196-BCE1-0F54EC92EC33}">
-  <dimension ref="A1:B61"/>
+  <dimension ref="A1:B62"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B61"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -11293,7 +11781,7 @@
         <v>2012</v>
       </c>
       <c r="B4">
-        <v>0</v>
+        <v>-0.48463199296432402</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -11301,7 +11789,7 @@
         <v>2013</v>
       </c>
       <c r="B5">
-        <v>0</v>
+        <v>-0.44279476957698699</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -11309,7 +11797,7 @@
         <v>2014</v>
       </c>
       <c r="B6">
-        <v>0</v>
+        <v>-0.39501557684159466</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -11317,7 +11805,7 @@
         <v>2015</v>
       </c>
       <c r="B7">
-        <v>0</v>
+        <v>-0.37898938142570604</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -11325,7 +11813,7 @@
         <v>2016</v>
       </c>
       <c r="B8">
-        <v>0</v>
+        <v>-0.35746845133604671</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -11333,7 +11821,7 @@
         <v>2017</v>
       </c>
       <c r="B9">
-        <v>0</v>
+        <v>-0.33551640350223444</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -11341,7 +11829,7 @@
         <v>2018</v>
       </c>
       <c r="B10">
-        <v>0</v>
+        <v>-0.31611792786789245</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -11349,7 +11837,7 @@
         <v>2019</v>
       </c>
       <c r="B11">
-        <v>0</v>
+        <v>-0.29419113555012588</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -11357,7 +11845,7 @@
         <v>2020</v>
       </c>
       <c r="B12">
-        <v>0</v>
+        <v>-0.275174972273524</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -11365,7 +11853,7 @@
         <v>2021</v>
       </c>
       <c r="B13">
-        <v>0</v>
+        <v>-0.25957357188884783</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -11373,7 +11861,7 @@
         <v>2022</v>
       </c>
       <c r="B14">
-        <v>0</v>
+        <v>-0.2522555041315423</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -11381,7 +11869,7 @@
         <v>2023</v>
       </c>
       <c r="B15">
-        <v>0</v>
+        <v>-0.2484037751560034</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -11389,7 +11877,7 @@
         <v>2024</v>
       </c>
       <c r="B16">
-        <v>0</v>
+        <v>-0.24178593173429327</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -11397,7 +11885,7 @@
         <v>2025</v>
       </c>
       <c r="B17">
-        <v>0</v>
+        <v>-0.24449858212979714</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -11405,7 +11893,7 @@
         <v>2026</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>-0.24903198566118756</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -11413,7 +11901,7 @@
         <v>2027</v>
       </c>
       <c r="B19">
-        <v>0</v>
+        <v>-0.25264201070565656</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -11421,7 +11909,7 @@
         <v>2028</v>
       </c>
       <c r="B20">
-        <v>0</v>
+        <v>-0.25364233752894055</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -11429,7 +11917,7 @@
         <v>2029</v>
       </c>
       <c r="B21">
-        <v>0</v>
+        <v>-0.24768152163486329</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -11437,7 +11925,7 @@
         <v>2030</v>
       </c>
       <c r="B22">
-        <v>0</v>
+        <v>-0.24974442678892514</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -11445,7 +11933,7 @@
         <v>2031</v>
       </c>
       <c r="B23">
-        <v>0</v>
+        <v>-0.24926794764317603</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -11453,7 +11941,7 @@
         <v>2032</v>
       </c>
       <c r="B24">
-        <v>0</v>
+        <v>-0.250134489952685</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -11461,7 +11949,7 @@
         <v>2033</v>
       </c>
       <c r="B25">
-        <v>0</v>
+        <v>-0.25159703697288732</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -11469,7 +11957,7 @@
         <v>2034</v>
       </c>
       <c r="B26">
-        <v>0</v>
+        <v>-0.25383394104860174</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -11477,7 +11965,7 @@
         <v>2035</v>
       </c>
       <c r="B27">
-        <v>0</v>
+        <v>-0.26016905205776741</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -11485,7 +11973,7 @@
         <v>2036</v>
       </c>
       <c r="B28">
-        <v>0</v>
+        <v>-0.27274303604096028</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -11493,7 +11981,7 @@
         <v>2037</v>
       </c>
       <c r="B29">
-        <v>0</v>
+        <v>-0.27650991999973468</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -11501,7 +11989,7 @@
         <v>2038</v>
       </c>
       <c r="B30">
-        <v>0</v>
+        <v>-0.28460685361503957</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -11509,7 +11997,7 @@
         <v>2039</v>
       </c>
       <c r="B31">
-        <v>0</v>
+        <v>-0.29665890398267214</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -11517,7 +12005,7 @@
         <v>2040</v>
       </c>
       <c r="B32">
-        <v>0</v>
+        <v>-0.30980188741828268</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -11525,7 +12013,7 @@
         <v>2041</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>-0.3249147353451094</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -11533,7 +12021,7 @@
         <v>2042</v>
       </c>
       <c r="B34">
-        <v>0</v>
+        <v>-0.33013144629608343</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -11541,7 +12029,7 @@
         <v>2043</v>
       </c>
       <c r="B35">
-        <v>0</v>
+        <v>-0.33400456174430643</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -11549,7 +12037,7 @@
         <v>2044</v>
       </c>
       <c r="B36">
-        <v>0</v>
+        <v>-0.34264176458383305</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -11557,7 +12045,7 @@
         <v>2045</v>
       </c>
       <c r="B37">
-        <v>0</v>
+        <v>-0.34821267929122846</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -11565,7 +12053,7 @@
         <v>2046</v>
       </c>
       <c r="B38">
-        <v>0</v>
+        <v>-0.34456161150133158</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -11573,7 +12061,7 @@
         <v>2047</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>-0.34561532498119613</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -11581,7 +12069,7 @@
         <v>2048</v>
       </c>
       <c r="B40">
-        <v>0</v>
+        <v>-0.33873736519970848</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -11589,7 +12077,7 @@
         <v>2049</v>
       </c>
       <c r="B41">
-        <v>0</v>
+        <v>-0.33739651765499096</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -11597,7 +12085,7 @@
         <v>2050</v>
       </c>
       <c r="B42">
-        <v>0</v>
+        <v>-0.33804860844064244</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -11605,7 +12093,7 @@
         <v>2051</v>
       </c>
       <c r="B43">
-        <v>0</v>
+        <v>-0.33657044977191414</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -11613,7 +12101,7 @@
         <v>2052</v>
       </c>
       <c r="B44">
-        <v>0</v>
+        <v>-0.33656675024980498</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -11621,7 +12109,7 @@
         <v>2053</v>
       </c>
       <c r="B45">
-        <v>0</v>
+        <v>-0.33985483078933226</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -11629,7 +12117,7 @@
         <v>2054</v>
       </c>
       <c r="B46">
-        <v>0</v>
+        <v>-0.33668670713123178</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -11637,7 +12125,7 @@
         <v>2055</v>
       </c>
       <c r="B47">
-        <v>0</v>
+        <v>-0.33750504731956005</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -11645,7 +12133,7 @@
         <v>2056</v>
       </c>
       <c r="B48">
-        <v>0</v>
+        <v>-0.34079779337557842</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -11653,7 +12141,7 @@
         <v>2057</v>
       </c>
       <c r="B49">
-        <v>0</v>
+        <v>-0.33872371122332023</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -11661,7 +12149,7 @@
         <v>2058</v>
       </c>
       <c r="B50">
-        <v>0</v>
+        <v>-0.33869137298543883</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -11669,7 +12157,7 @@
         <v>2059</v>
       </c>
       <c r="B51">
-        <v>0</v>
+        <v>-0.34103219793504497</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -11677,7 +12165,7 @@
         <v>2060</v>
       </c>
       <c r="B52">
-        <v>0</v>
+        <v>-0.34050601889900228</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -11685,7 +12173,7 @@
         <v>2061</v>
       </c>
       <c r="B53">
-        <v>0</v>
+        <v>-0.33767373591580502</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -11693,7 +12181,7 @@
         <v>2062</v>
       </c>
       <c r="B54">
-        <v>0</v>
+        <v>-0.33668796343699775</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -11701,7 +12189,7 @@
         <v>2063</v>
       </c>
       <c r="B55">
-        <v>0</v>
+        <v>-0.33369114324283816</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -11709,7 +12197,7 @@
         <v>2064</v>
       </c>
       <c r="B56">
-        <v>0</v>
+        <v>-0.33282968867461227</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -11717,7 +12205,7 @@
         <v>2065</v>
       </c>
       <c r="B57">
-        <v>0</v>
+        <v>-0.32675564471673357</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -11725,7 +12213,7 @@
         <v>2066</v>
       </c>
       <c r="B58">
-        <v>0</v>
+        <v>-0.32143826156637562</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -11733,7 +12221,7 @@
         <v>2067</v>
       </c>
       <c r="B59">
-        <v>0</v>
+        <v>-0.31711471655916201</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -11741,7 +12229,7 @@
         <v>2068</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>-0.31670999077073719</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -11749,7 +12237,15 @@
         <v>2069</v>
       </c>
       <c r="B61">
-        <v>0</v>
+        <v>-0.31670999077073719</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <v>2070</v>
+      </c>
+      <c r="B62">
+        <v>-0.31670999077073719</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
slight improvement of messages
</commit_message>
<xml_diff>
--- a/input/time_series_factor.xlsx
+++ b/input/time_series_factor.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MyFiles\99 DEV ENV\JAS-MINE\SimPaths\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097CE548-6F17-4B75-8319-73D61F0113A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7EC5005-AAD9-4E8B-AC05-A7C58FC4F3F9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -35,18 +35,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="56">
   <si>
     <t>Year</t>
   </si>
@@ -208,6 +202,12 @@
   </si>
   <si>
     <t>GDP CVMs (real)</t>
+  </si>
+  <si>
+    <t>standard model</t>
+  </si>
+  <si>
+    <t>dynamic utility model</t>
   </si>
 </sst>
 </file>
@@ -11237,506 +11237,880 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D18E90C-6D91-4744-9FCB-A05B59544AB8}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
       <c r="B4">
+        <v>-0.68042582690000331</v>
+      </c>
+      <c r="E4">
         <v>-0.95768509819680903</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>-0.68042582690000331</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
       <c r="B5">
+        <v>-0.67229930191496556</v>
+      </c>
+      <c r="E5">
         <v>-0.83295781453007001</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>-0.67229930191496556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
       <c r="B6">
+        <v>-0.67897363322872639</v>
+      </c>
+      <c r="E6">
         <v>-0.80485660959326355</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>-0.67897363322872639</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
       <c r="B7">
+        <v>-0.66203073162886494</v>
+      </c>
+      <c r="E7">
         <v>-0.78981867057924415</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>-0.66203073162886494</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2016</v>
       </c>
       <c r="B8">
+        <v>-0.65127749552133463</v>
+      </c>
+      <c r="E8">
         <v>-0.77794475503792282</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>-0.65127749552133463</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>
       <c r="B9">
+        <v>-0.62856645997943639</v>
+      </c>
+      <c r="E9">
         <v>-0.75171647264083308</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>-0.62856645997943639</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
       <c r="B10">
+        <v>-0.62262883931939683</v>
+      </c>
+      <c r="E10">
         <v>-0.74109647439251236</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>-0.62262883931939683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2019</v>
       </c>
       <c r="B11">
+        <v>-0.61386966551793498</v>
+      </c>
+      <c r="E11">
         <v>-0.72776510107134573</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>-0.61386966551793498</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
       <c r="B12">
+        <v>-0.59884444696646777</v>
+      </c>
+      <c r="E12">
         <v>-0.7147060419149136</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>-0.59884444696646777</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2021</v>
       </c>
       <c r="B13">
+        <v>-0.58212592838721533</v>
+      </c>
+      <c r="E13">
         <v>-0.70240616614065376</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>-0.58212592838721533</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2022</v>
       </c>
       <c r="B14">
+        <v>-0.58476026852042595</v>
+      </c>
+      <c r="E14">
         <v>-0.69105367590666433</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>-0.58476026852042595</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2023</v>
       </c>
       <c r="B15">
+        <v>-0.56894577426477011</v>
+      </c>
+      <c r="E15">
         <v>-0.67898522305967135</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>-0.56894577426477011</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2024</v>
       </c>
       <c r="B16">
+        <v>-0.55774239163231498</v>
+      </c>
+      <c r="E16">
         <v>-0.67837200227633576</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>-0.55774239163231498</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2025</v>
       </c>
       <c r="B17">
+        <v>-0.5546484315400706</v>
+      </c>
+      <c r="E17">
         <v>-0.66865521484219381</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>-0.5546484315400706</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2026</v>
       </c>
       <c r="B18">
+        <v>-0.54633744534475526</v>
+      </c>
+      <c r="E18">
         <v>-0.66213777125088935</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>-0.54633744534475526</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2027</v>
       </c>
       <c r="B19">
+        <v>-0.53660398326743075</v>
+      </c>
+      <c r="E19">
         <v>-0.65624918555298262</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>-0.53660398326743075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2028</v>
       </c>
       <c r="B20">
+        <v>-0.52636891781716488</v>
+      </c>
+      <c r="E20">
         <v>-0.65247439548232655</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>-0.52636891781716488</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2029</v>
       </c>
       <c r="B21">
+        <v>-0.52739427357167223</v>
+      </c>
+      <c r="E21">
         <v>-0.64776174741668557</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>-0.52739427357167223</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2030</v>
       </c>
       <c r="B22">
+        <v>-0.522335868711721</v>
+      </c>
+      <c r="E22">
         <v>-0.64184148070049241</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>-0.522335868711721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2031</v>
       </c>
       <c r="B23">
+        <v>-0.51932161850484515</v>
+      </c>
+      <c r="E23">
         <v>-0.63931566276826524</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>-0.51932161850484515</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2032</v>
       </c>
       <c r="B24">
+        <v>-0.51851186880903399</v>
+      </c>
+      <c r="E24">
         <v>-0.63638760354965007</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>-0.51851186880903399</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2033</v>
       </c>
       <c r="B25">
+        <v>-0.52248458236888451</v>
+      </c>
+      <c r="E25">
         <v>-0.63218797948615213</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>-0.52248458236888451</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2034</v>
       </c>
       <c r="B26">
+        <v>-0.51756454907723248</v>
+      </c>
+      <c r="E26">
         <v>-0.62979949109872213</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>-0.51756454907723248</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2035</v>
       </c>
       <c r="B27">
+        <v>-0.51707659305484055</v>
+      </c>
+      <c r="E27">
         <v>-0.62642840586058846</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>-0.51707659305484055</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2036</v>
       </c>
       <c r="B28">
+        <v>-0.51785189045280133</v>
+      </c>
+      <c r="E28">
         <v>-0.62703195252281929</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>-0.51785189045280133</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2037</v>
       </c>
       <c r="B29">
+        <v>-0.52133458277805855</v>
+      </c>
+      <c r="E29">
         <v>-0.62763592693798487</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>-0.52133458277805855</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2038</v>
       </c>
       <c r="B30">
+        <v>-0.52255964231049601</v>
+      </c>
+      <c r="E30">
         <v>-0.62901387736233438</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>-0.52255964231049601</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2039</v>
       </c>
       <c r="B31">
+        <v>-0.52461978177447943</v>
+      </c>
+      <c r="E31">
         <v>-0.62870490298773551</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>-0.52461978177447943</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2040</v>
       </c>
       <c r="B32">
+        <v>-0.52602689591038243</v>
+      </c>
+      <c r="E32">
         <v>-0.63132275325212173</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>-0.52602689591038243</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2041</v>
       </c>
       <c r="B33">
+        <v>-0.52818471105801446</v>
+      </c>
+      <c r="E33">
         <v>-0.63189417814259741</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>-0.52818471105801446</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2042</v>
       </c>
       <c r="B34">
+        <v>-0.52582640158760352</v>
+      </c>
+      <c r="E34">
         <v>-0.63431628626780423</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>-0.52582640158760352</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2043</v>
       </c>
       <c r="B35">
+        <v>-0.52884537398341225</v>
+      </c>
+      <c r="E35">
         <v>-0.63319756552905415</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>-0.52884537398341225</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2044</v>
       </c>
       <c r="B36">
+        <v>-0.53136207561516069</v>
+      </c>
+      <c r="E36">
         <v>-0.63471667603087323</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>-0.53136207561516069</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2045</v>
       </c>
       <c r="B37">
+        <v>-0.53392813259970762</v>
+      </c>
+      <c r="E37">
         <v>-0.63455648067220116</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>-0.53392813259970762</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2046</v>
       </c>
       <c r="B38">
+        <v>-0.53502526357346303</v>
+      </c>
+      <c r="E38">
         <v>-0.63527012935003857</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>-0.53502526357346303</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2047</v>
       </c>
       <c r="B39">
+        <v>-0.5361827911656164</v>
+      </c>
+      <c r="E39">
         <v>-0.63488663198137396</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>-0.5361827911656164</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2048</v>
       </c>
       <c r="B40">
+        <v>-0.53742998980006962</v>
+      </c>
+      <c r="E40">
         <v>-0.6327623871436846</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>-0.53742998980006962</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2049</v>
       </c>
       <c r="B41">
+        <v>-0.53265366720456808</v>
+      </c>
+      <c r="E41">
         <v>-0.63172645653828041</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>-0.53265366720456808</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2050</v>
       </c>
       <c r="B42">
+        <v>-0.52672262067763742</v>
+      </c>
+      <c r="E42">
         <v>-0.63131309782462763</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>-0.52672262067763742</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2051</v>
       </c>
       <c r="B43">
+        <v>-0.52246561759781496</v>
+      </c>
+      <c r="E43">
         <v>-0.62711212192261312</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>-0.52246561759781496</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2052</v>
       </c>
       <c r="B44">
+        <v>-0.51992475724234222</v>
+      </c>
+      <c r="E44">
         <v>-0.62483324297863929</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>-0.51992475724234222</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2053</v>
       </c>
       <c r="B45">
+        <v>-0.51600574555924328</v>
+      </c>
+      <c r="E45">
         <v>-0.62289315139452228</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>-0.51600574555924328</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2054</v>
       </c>
       <c r="B46">
+        <v>-0.51576972424348644</v>
+      </c>
+      <c r="E46">
         <v>-0.6208575795852076</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>-0.51576972424348644</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2055</v>
       </c>
       <c r="B47">
+        <v>-0.51800776098642443</v>
+      </c>
+      <c r="E47">
         <v>-0.62046331508145192</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>-0.51800776098642443</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2056</v>
       </c>
       <c r="B48">
+        <v>-0.51952270196948724</v>
+      </c>
+      <c r="E48">
         <v>-0.61860426418741976</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>-0.51952270196948724</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2057</v>
       </c>
       <c r="B49">
+        <v>-0.52097143042496585</v>
+      </c>
+      <c r="E49">
         <v>-0.61533367788355553</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>-0.52097143042496585</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2058</v>
       </c>
       <c r="B50">
+        <v>-0.51855272309252176</v>
+      </c>
+      <c r="E50">
         <v>-0.61489963029454253</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>-0.51855272309252176</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2059</v>
       </c>
       <c r="B51">
+        <v>-0.51809916084156005</v>
+      </c>
+      <c r="E51">
         <v>-0.61364330813003531</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>-0.51809916084156005</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2060</v>
       </c>
       <c r="B52">
+        <v>-0.51977389607061364</v>
+      </c>
+      <c r="E52">
         <v>-0.61242239408296961</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>-0.51977389607061364</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2061</v>
       </c>
       <c r="B53">
+        <v>-0.51599900885427696</v>
+      </c>
+      <c r="E53">
         <v>-0.61091556383364465</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>-0.51599900885427696</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2062</v>
       </c>
       <c r="B54">
+        <v>-0.51480700328602169</v>
+      </c>
+      <c r="E54">
         <v>-0.60932285274850906</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>-0.51480700328602169</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2063</v>
       </c>
       <c r="B55">
+        <v>-0.51568068499828201</v>
+      </c>
+      <c r="E55">
         <v>-0.60791630071486702</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>-0.51568068499828201</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2064</v>
       </c>
       <c r="B56">
+        <v>-0.51597773825575943</v>
+      </c>
+      <c r="E56">
         <v>-0.60902347078757146</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>-0.51597773825575943</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2065</v>
       </c>
       <c r="B57">
+        <v>-0.50918163905100955</v>
+      </c>
+      <c r="E57">
         <v>-0.60734177454365323</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>-0.50918163905100955</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2066</v>
       </c>
       <c r="B58">
+        <v>-0.51037220329257249</v>
+      </c>
+      <c r="E58">
         <v>-0.60672079418846891</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>-0.51037220329257249</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2067</v>
       </c>
       <c r="B59">
+        <v>-0.50578085391324401</v>
+      </c>
+      <c r="E59">
         <v>-0.6058496118125366</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>-0.50578085391324401</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2068</v>
       </c>
       <c r="B60">
+        <v>-0.50041296740445906</v>
+      </c>
+      <c r="E60">
         <v>-0.60652410750329455</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>-0.50041296740445906</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2069</v>
       </c>
       <c r="B61">
+        <v>-0.50041296740445906</v>
+      </c>
+      <c r="E61">
         <v>-0.60652410750329455</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>-0.50041296740445906</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2070</v>
       </c>
       <c r="B62">
+        <v>-0.50041296740445906</v>
+      </c>
+      <c r="E62">
         <v>-0.60652410750329455</v>
+      </c>
+      <c r="F62">
+        <v>-0.50041296740445906</v>
       </c>
     </row>
   </sheetData>
@@ -11746,506 +12120,880 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B00E6D01-ED8F-4196-BCE1-0F54EC92EC33}">
-  <dimension ref="A1:B62"/>
+  <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B62"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2010</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2011</v>
       </c>
       <c r="B3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2012</v>
       </c>
       <c r="B4">
+        <v>-0.44081411312763502</v>
+      </c>
+      <c r="E4">
         <v>-0.48463199296432402</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>-0.44081411312763502</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2013</v>
       </c>
       <c r="B5">
+        <v>-0.41178003442893141</v>
+      </c>
+      <c r="E5">
         <v>-0.44279476957698699</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>-0.41178003442893141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2014</v>
       </c>
       <c r="B6">
+        <v>-0.38195691653651342</v>
+      </c>
+      <c r="E6">
         <v>-0.39501557684159466</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>-0.38195691653651342</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2015</v>
       </c>
       <c r="B7">
+        <v>-0.35662154819469444</v>
+      </c>
+      <c r="E7">
         <v>-0.37898938142570604</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>-0.35662154819469444</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2016</v>
       </c>
       <c r="B8">
+        <v>-0.33645665993640061</v>
+      </c>
+      <c r="E8">
         <v>-0.35746845133604671</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>-0.33645665993640061</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2017</v>
       </c>
       <c r="B9">
+        <v>-0.31569377810596422</v>
+      </c>
+      <c r="E9">
         <v>-0.33551640350223444</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>-0.31569377810596422</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2018</v>
       </c>
       <c r="B10">
+        <v>-0.29611480221652442</v>
+      </c>
+      <c r="E10">
         <v>-0.31611792786789245</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>-0.29611480221652442</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2019</v>
       </c>
       <c r="B11">
+        <v>-0.279462622342386</v>
+      </c>
+      <c r="E11">
         <v>-0.29419113555012588</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>-0.279462622342386</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2020</v>
       </c>
       <c r="B12">
+        <v>-0.26591979180000819</v>
+      </c>
+      <c r="E12">
         <v>-0.275174972273524</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>-0.26591979180000819</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2021</v>
       </c>
       <c r="B13">
+        <v>-0.25543875103684177</v>
+      </c>
+      <c r="E13">
         <v>-0.25957357188884783</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>-0.25543875103684177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2022</v>
       </c>
       <c r="B14">
+        <v>-0.24930347300809638</v>
+      </c>
+      <c r="E14">
         <v>-0.2522555041315423</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>-0.24930347300809638</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2023</v>
       </c>
       <c r="B15">
+        <v>-0.2471951557625644</v>
+      </c>
+      <c r="E15">
         <v>-0.2484037751560034</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>-0.2471951557625644</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2024</v>
       </c>
       <c r="B16">
+        <v>-0.24727245707738721</v>
+      </c>
+      <c r="E16">
         <v>-0.24178593173429327</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F16">
+        <v>-0.24727245707738721</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2025</v>
       </c>
       <c r="B17">
+        <v>-0.23666450179745918</v>
+      </c>
+      <c r="E17">
         <v>-0.24449858212979714</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F17">
+        <v>-0.23666450179745918</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2026</v>
       </c>
       <c r="B18">
+        <v>-0.23784361977757321</v>
+      </c>
+      <c r="E18">
         <v>-0.24903198566118756</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F18">
+        <v>-0.23784361977757321</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2027</v>
       </c>
       <c r="B19">
+        <v>-0.23889278870939884</v>
+      </c>
+      <c r="E19">
         <v>-0.25264201070565656</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>-0.23889278870939884</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2028</v>
       </c>
       <c r="B20">
+        <v>-0.23893998110579662</v>
+      </c>
+      <c r="E20">
         <v>-0.25364233752894055</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F20">
+        <v>-0.23893998110579662</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2029</v>
       </c>
       <c r="B21">
+        <v>-0.23843847695520243</v>
+      </c>
+      <c r="E21">
         <v>-0.24768152163486329</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F21">
+        <v>-0.23843847695520243</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2030</v>
       </c>
       <c r="B22">
+        <v>-0.24968508459850719</v>
+      </c>
+      <c r="E22">
         <v>-0.24974442678892514</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F22">
+        <v>-0.24968508459850719</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2031</v>
       </c>
       <c r="B23">
+        <v>-0.25091556848125485</v>
+      </c>
+      <c r="E23">
         <v>-0.24926794764317603</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F23">
+        <v>-0.25091556848125485</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2032</v>
       </c>
       <c r="B24">
+        <v>-0.25300049353502324</v>
+      </c>
+      <c r="E24">
         <v>-0.250134489952685</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F24">
+        <v>-0.25300049353502324</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2033</v>
       </c>
       <c r="B25">
+        <v>-0.25769551121458001</v>
+      </c>
+      <c r="E25">
         <v>-0.25159703697288732</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F25">
+        <v>-0.25769551121458001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2034</v>
       </c>
       <c r="B26">
+        <v>-0.26297059722398985</v>
+      </c>
+      <c r="E26">
         <v>-0.25383394104860174</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F26">
+        <v>-0.26297059722398985</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2035</v>
       </c>
       <c r="B27">
+        <v>-0.26957256055242024</v>
+      </c>
+      <c r="E27">
         <v>-0.26016905205776741</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F27">
+        <v>-0.26957256055242024</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2036</v>
       </c>
       <c r="B28">
+        <v>-0.27813755313923438</v>
+      </c>
+      <c r="E28">
         <v>-0.27274303604096028</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F28">
+        <v>-0.27813755313923438</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2037</v>
       </c>
       <c r="B29">
+        <v>-0.27474637053283057</v>
+      </c>
+      <c r="E29">
         <v>-0.27650991999973468</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F29">
+        <v>-0.27474637053283057</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2038</v>
       </c>
       <c r="B30">
+        <v>-0.28518071039366039</v>
+      </c>
+      <c r="E30">
         <v>-0.28460685361503957</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F30">
+        <v>-0.28518071039366039</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2039</v>
       </c>
       <c r="B31">
+        <v>-0.2959050156529302</v>
+      </c>
+      <c r="E31">
         <v>-0.29665890398267214</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F31">
+        <v>-0.2959050156529302</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2040</v>
       </c>
       <c r="B32">
+        <v>-0.2928526070865794</v>
+      </c>
+      <c r="E32">
         <v>-0.30980188741828268</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F32">
+        <v>-0.2928526070865794</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2041</v>
       </c>
       <c r="B33">
+        <v>-0.30204917920681157</v>
+      </c>
+      <c r="E33">
         <v>-0.3249147353451094</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F33">
+        <v>-0.30204917920681157</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2042</v>
       </c>
       <c r="B34">
+        <v>-0.32304908725990761</v>
+      </c>
+      <c r="E34">
         <v>-0.33013144629608343</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F34">
+        <v>-0.32304908725990761</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2043</v>
       </c>
       <c r="B35">
+        <v>-0.32697846249115198</v>
+      </c>
+      <c r="E35">
         <v>-0.33400456174430643</v>
       </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F35">
+        <v>-0.32697846249115198</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2044</v>
       </c>
       <c r="B36">
+        <v>-0.33007523822817458</v>
+      </c>
+      <c r="E36">
         <v>-0.34264176458383305</v>
       </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F36">
+        <v>-0.33007523822817458</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2045</v>
       </c>
       <c r="B37">
+        <v>-0.34395374911145921</v>
+      </c>
+      <c r="E37">
         <v>-0.34821267929122846</v>
       </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F37">
+        <v>-0.34395374911145921</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2046</v>
       </c>
       <c r="B38">
+        <v>-0.32911187304579681</v>
+      </c>
+      <c r="E38">
         <v>-0.34456161150133158</v>
       </c>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F38">
+        <v>-0.32911187304579681</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2047</v>
       </c>
       <c r="B39">
+        <v>-0.32707905887567962</v>
+      </c>
+      <c r="E39">
         <v>-0.34561532498119613</v>
       </c>
-    </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F39">
+        <v>-0.32707905887567962</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2048</v>
       </c>
       <c r="B40">
+        <v>-0.32548082652979621</v>
+      </c>
+      <c r="E40">
         <v>-0.33873736519970848</v>
       </c>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F40">
+        <v>-0.32548082652979621</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2049</v>
       </c>
       <c r="B41">
+        <v>-0.32367111158351802</v>
+      </c>
+      <c r="E41">
         <v>-0.33739651765499096</v>
       </c>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F41">
+        <v>-0.32367111158351802</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2050</v>
       </c>
       <c r="B42">
+        <v>-0.31183478961522498</v>
+      </c>
+      <c r="E42">
         <v>-0.33804860844064244</v>
       </c>
-    </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F42">
+        <v>-0.31183478961522498</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2051</v>
       </c>
       <c r="B43">
+        <v>-0.30933783525634517</v>
+      </c>
+      <c r="E43">
         <v>-0.33657044977191414</v>
       </c>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F43">
+        <v>-0.30933783525634517</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2052</v>
       </c>
       <c r="B44">
+        <v>-0.295502572399851</v>
+      </c>
+      <c r="E44">
         <v>-0.33656675024980498</v>
       </c>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F44">
+        <v>-0.295502572399851</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2053</v>
       </c>
       <c r="B45">
+        <v>-0.28426566851705959</v>
+      </c>
+      <c r="E45">
         <v>-0.33985483078933226</v>
       </c>
-    </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F45">
+        <v>-0.28426566851705959</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2054</v>
       </c>
       <c r="B46">
+        <v>-0.2846970607117626</v>
+      </c>
+      <c r="E46">
         <v>-0.33668670713123178</v>
       </c>
-    </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F46">
+        <v>-0.2846970607117626</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2055</v>
       </c>
       <c r="B47">
+        <v>-0.29652418423720162</v>
+      </c>
+      <c r="E47">
         <v>-0.33750504731956005</v>
       </c>
-    </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F47">
+        <v>-0.29652418423720162</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2056</v>
       </c>
       <c r="B48">
+        <v>-0.31354110133198604</v>
+      </c>
+      <c r="E48">
         <v>-0.34079779337557842</v>
       </c>
-    </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F48">
+        <v>-0.31354110133198604</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2057</v>
       </c>
       <c r="B49">
+        <v>-0.3278678462801522</v>
+      </c>
+      <c r="E49">
         <v>-0.33872371122332023</v>
       </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F49">
+        <v>-0.3278678462801522</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2058</v>
       </c>
       <c r="B50">
+        <v>-0.33932540739172184</v>
+      </c>
+      <c r="E50">
         <v>-0.33869137298543883</v>
       </c>
-    </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F50">
+        <v>-0.33932540739172184</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2059</v>
       </c>
       <c r="B51">
+        <v>-0.33891825783445723</v>
+      </c>
+      <c r="E51">
         <v>-0.34103219793504497</v>
       </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F51">
+        <v>-0.33891825783445723</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2060</v>
       </c>
       <c r="B52">
+        <v>-0.33791821188593724</v>
+      </c>
+      <c r="E52">
         <v>-0.34050601889900228</v>
       </c>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F52">
+        <v>-0.33791821188593724</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2061</v>
       </c>
       <c r="B53">
+        <v>-0.33627771003385082</v>
+      </c>
+      <c r="E53">
         <v>-0.33767373591580502</v>
       </c>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F53">
+        <v>-0.33627771003385082</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2062</v>
       </c>
       <c r="B54">
+        <v>-0.33352763519739703</v>
+      </c>
+      <c r="E54">
         <v>-0.33668796343699775</v>
       </c>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F54">
+        <v>-0.33352763519739703</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2063</v>
       </c>
       <c r="B55">
+        <v>-0.33028054032751103</v>
+      </c>
+      <c r="E55">
         <v>-0.33369114324283816</v>
       </c>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>-0.33028054032751103</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2064</v>
       </c>
       <c r="B56">
+        <v>-0.32636589095194396</v>
+      </c>
+      <c r="E56">
         <v>-0.33282968867461227</v>
       </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>-0.32636589095194396</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2065</v>
       </c>
       <c r="B57">
+        <v>-0.32296966045752384</v>
+      </c>
+      <c r="E57">
         <v>-0.32675564471673357</v>
       </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F57">
+        <v>-0.32296966045752384</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2066</v>
       </c>
       <c r="B58">
+        <v>-0.3197457208767488</v>
+      </c>
+      <c r="E58">
         <v>-0.32143826156637562</v>
       </c>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F58">
+        <v>-0.3197457208767488</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2067</v>
       </c>
       <c r="B59">
+        <v>-0.31773659008754962</v>
+      </c>
+      <c r="E59">
         <v>-0.31711471655916201</v>
       </c>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F59">
+        <v>-0.31773659008754962</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2068</v>
       </c>
       <c r="B60">
+        <v>-0.31670999077073703</v>
+      </c>
+      <c r="E60">
         <v>-0.31670999077073719</v>
       </c>
-    </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F60">
+        <v>-0.31670999077073703</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2069</v>
       </c>
       <c r="B61">
+        <v>-0.31670999077073703</v>
+      </c>
+      <c r="E61">
         <v>-0.31670999077073719</v>
       </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="F61">
+        <v>-0.31670999077073703</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2070</v>
       </c>
       <c r="B62">
+        <v>-0.31670999077073703</v>
+      </c>
+      <c r="E62">
         <v>-0.31670999077073719</v>
+      </c>
+      <c r="F62">
+        <v>-0.31670999077073703</v>
       </c>
     </row>
   </sheetData>

</xml_diff>